<commit_message>
Finished with DfFroc2Roc code
1. Test wAfroc and Wilcoxon FOMs in jackknife code
2. Using arrays simplifies the jackknife code
3. Checked out array indexing code with JT dataset with wAfroc FOM
4. Finished with DfFroc2Roc code

The deep copy vs shallow copy is a nasty Python concept :(

https://www.quora.com/Why-is-default-Python-assignment-a-shallow-copy-when-it-seems-that-itd-be-more-often-problematic-than-helpful
</commit_message>
<xml_diff>
--- a/Py/extdata/toyFiles/ROC/rocCr.xlsx
+++ b/Py/extdata/toyFiles/ROC/rocCr.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/ROC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/Py/extdata/toyFiles/ROC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7984E2AB-3BCF-A14D-B0DE-FCF45F77A828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C8C964-F54C-A045-8E21-264D2DC79359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16420" yWindow="460" windowWidth="10000" windowHeight="10140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FP" sheetId="2" r:id="rId1"/>
-    <sheet name="TP" sheetId="3" r:id="rId2"/>
+    <sheet name="NL" sheetId="2" r:id="rId1"/>
+    <sheet name="LL" sheetId="3" r:id="rId2"/>
     <sheet name="TRUTH" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="12">
   <si>
     <t>CaseID</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>ModalityID</t>
-  </si>
-  <si>
-    <t>FP_Rating</t>
   </si>
   <si>
     <t>0</t>
@@ -62,22 +59,10 @@
     <t>4</t>
   </si>
   <si>
-    <t>0,1,2,3,4</t>
+    <t>NLRating</t>
   </si>
   <si>
-    <t>TP_Rating</t>
-  </si>
-  <si>
-    <t>Paradigm</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>ROC</t>
-  </si>
-  <si>
-    <t>FCTRL</t>
+    <t>LLRating</t>
   </si>
 </sst>
 </file>
@@ -481,7 +466,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -501,15 +486,15 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -520,10 +505,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -534,10 +519,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -548,10 +533,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -562,10 +547,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -576,10 +561,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -590,10 +575,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -604,10 +589,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -618,10 +603,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -632,10 +617,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -646,10 +631,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -660,10 +645,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -674,10 +659,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -688,10 +673,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -702,10 +687,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -716,10 +701,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -730,10 +715,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -744,10 +729,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -758,10 +743,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -772,10 +757,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -786,10 +771,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -800,10 +785,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -814,10 +799,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -828,10 +813,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
@@ -842,10 +827,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -856,10 +841,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -870,10 +855,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -884,10 +869,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -898,10 +883,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
@@ -912,10 +897,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -942,7 +927,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -965,15 +950,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>70</v>
@@ -987,10 +972,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>71</v>
@@ -1004,10 +989,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>72</v>
@@ -1021,10 +1006,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>73</v>
@@ -1038,10 +1023,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>74</v>
@@ -1055,10 +1040,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>70</v>
@@ -1072,10 +1057,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>71</v>
@@ -1089,10 +1074,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>72</v>
@@ -1106,10 +1091,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>73</v>
@@ -1123,10 +1108,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>74</v>
@@ -1140,10 +1125,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>70</v>
@@ -1157,10 +1142,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>71</v>
@@ -1174,10 +1159,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>72</v>
@@ -1191,10 +1176,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>73</v>
@@ -1208,10 +1193,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>74</v>
@@ -1225,10 +1210,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>70</v>
@@ -1242,10 +1227,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>71</v>
@@ -1259,10 +1244,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>72</v>
@@ -1276,10 +1261,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>73</v>
@@ -1293,10 +1278,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>74</v>
@@ -1310,10 +1295,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1">
         <v>70</v>
@@ -1327,10 +1312,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
         <v>71</v>
@@ -1344,10 +1329,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1">
         <v>72</v>
@@ -1361,10 +1346,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1">
         <v>73</v>
@@ -1378,10 +1363,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1">
         <v>74</v>
@@ -1395,10 +1380,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>70</v>
@@ -1412,10 +1397,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <v>71</v>
@@ -1429,10 +1414,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>72</v>
@@ -1446,10 +1431,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>73</v>
@@ -1463,10 +1448,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1">
         <v>74</v>
@@ -1480,10 +1465,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1">
         <v>70</v>
@@ -1497,10 +1482,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1">
         <v>71</v>
@@ -1514,10 +1499,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1">
         <v>72</v>
@@ -1531,10 +1516,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="1">
         <v>73</v>
@@ -1548,10 +1533,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1">
         <v>74</v>
@@ -1565,10 +1550,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1">
         <v>70</v>
@@ -1582,10 +1567,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38" s="1">
         <v>71</v>
@@ -1599,10 +1584,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="1">
         <v>72</v>
@@ -1616,10 +1601,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" s="1">
         <v>73</v>
@@ -1633,10 +1618,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1">
         <v>74</v>
@@ -1650,10 +1635,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" s="1">
         <v>70</v>
@@ -1667,10 +1652,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1">
         <v>71</v>
@@ -1684,10 +1669,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" s="1">
         <v>72</v>
@@ -1701,10 +1686,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45" s="1">
         <v>73</v>
@@ -1718,10 +1703,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" s="1">
         <v>74</v>
@@ -1735,10 +1720,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" s="1">
         <v>70</v>
@@ -1752,10 +1737,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48" s="1">
         <v>71</v>
@@ -1769,10 +1754,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1">
         <v>72</v>
@@ -1786,10 +1771,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" s="1">
         <v>73</v>
@@ -1803,10 +1788,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="1">
         <v>74</v>
@@ -1833,22 +1818,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1858,17 +1840,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1878,17 +1851,8 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1898,17 +1862,8 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1918,15 +1873,8 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>70</v>
       </c>
@@ -1936,15 +1884,8 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>71</v>
       </c>
@@ -1954,15 +1895,8 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>72</v>
       </c>
@@ -1972,15 +1906,8 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>73</v>
       </c>
@@ -1990,15 +1917,8 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>74</v>
       </c>
@@ -2008,29 +1928,6 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>